<commit_message>
added code to move old extent reports to archive Folder
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AE4C80B0-F631-4AA4-B911-C94D0E21031B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{485C680D-4A3F-4285-A0EB-77F01C0A3755}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="2925" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="69">
   <si>
     <t>endPoint</t>
   </si>
@@ -201,13 +201,37 @@
   </si>
   <si>
     <t>description:Customer for nisha@example.com</t>
+  </si>
+  <si>
+    <t>verifyCreateCharge</t>
+  </si>
+  <si>
+    <t>amount:100;currency:USD;source:tok_mastercard;description:This is to check the run for multiple params from same column</t>
+  </si>
+  <si>
+    <t>verifyRetrieveCharge</t>
+  </si>
+  <si>
+    <t>charges/ch_1DwmfkJ06AnIpd2yPPLsRCv9</t>
+  </si>
+  <si>
+    <t>verifyRetrieveAllCharge</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>charges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +259,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -257,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -269,6 +299,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -893,17 +927,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -923,7 +957,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -943,7 +977,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -960,10 +994,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,8 +1030,8 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>201</v>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1071,32 +1105,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1104,7 +1138,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1112,8 +1146,86 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>